<commit_message>
Add new url in vacancies. Add average points in Resume
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="9720" windowHeight="2790"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,12 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -129,33 +130,9 @@
     <t>prof</t>
   </si>
   <si>
-    <t>site1</t>
-  </si>
-  <si>
-    <t>https://rabota.by/</t>
-  </si>
-  <si>
     <t>urlForProf</t>
   </si>
   <si>
-    <t>https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;ored_clusters=true&amp;enable_snippets=true&amp;only_with_salary=true&amp;st=searchVacancy&amp;text=</t>
-  </si>
-  <si>
-    <t>site2</t>
-  </si>
-  <si>
-    <t>https://belmeta.com/vacansii?q=%D0%BA%D0%BB%D0%B0%D0%B4%D0%BE%D0%B2%D1%89%D0%B8%D0%BA&amp;l=%D0%9C%D0%B8%D0%BD%D1%81%D0%BA</t>
-  </si>
-  <si>
-    <t>https://belmeta.com/vacansii?q=&amp;l=Минск</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Указываем начало ячейки в выходном файле для записи результатов </t>
-  </si>
-  <si>
-    <t>Укладчик-упаковщик/Комплектовщик,B206;Кладовщик,B84;Продавец,B23;Слесарь-сантехник,B145;Официант,B267</t>
-  </si>
-  <si>
     <t>urlForSalesAss</t>
   </si>
   <si>
@@ -171,19 +148,37 @@
     <t>urlForUklUpak</t>
   </si>
   <si>
-    <t>https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;industry=5&amp;industry=42&amp;ored_clusters=true&amp;enable_snippets=true&amp;only_with_salary=true&amp;st=searchVacancy&amp;text=</t>
-  </si>
-  <si>
-    <t>Машинист котлов,B328;Оператор котельной,B389</t>
-  </si>
-  <si>
     <t>resumeURL</t>
   </si>
   <si>
-    <t>https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magic=true&amp;order_by=relevance&amp;ored_clusters=true&amp;search_period=30&amp;pos=position&amp;text=</t>
-  </si>
-  <si>
-    <t>Кладовщик,B84;Укладчик-упаковщик/Комплектовщик,B206;Продавец,B23;Слесарь-сантехник,B145;Официант,B267</t>
+    <t>https://rabota.by/search/resume?text="Подбор+персонала"+AND+Рекрутинг+AND+Recruiter&amp;logic=normal&amp;pos=education&amp;exp_period=all_time&amp;exp_company_size=any&amp;exp_industry=any&amp;area=1004&amp;relocation=living_or_relocation&amp;salary_from=&amp;salary_to=&amp;currency_code=BYR&amp;education=higher&amp;age_from=&amp;age_to=&amp;gender=unknown&amp;order_by=relevance&amp;search_period=0&amp;items_on_page=100&amp;no_magic=false</t>
+  </si>
+  <si>
+    <t>urlRecruiter</t>
+  </si>
+  <si>
+    <t>Указываем вакансия, начало ячейки в выходном файле для записи результатов, имя параметра в Эксель с урл для поиска</t>
+  </si>
+  <si>
+    <t>urlForSlesar</t>
+  </si>
+  <si>
+    <t>Кладовщик,B84,urlForStoreKpr;Укладчик-упаковщик/Комплектовщик,B206,urlForUklUpak;Продавец,B23,urlForSalesAss;Слесарь-сантехник,B145,urlForSlesar;Официант,B267,urlForProf</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;ored_clusters=true&amp;enable_snippets=true&amp;items_on_page=100&amp;only_with_salary=true&amp;st=searchVacancy&amp;search_field=name&amp;text=%21</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;items_on_page=100&amp;no_magic=true&amp;ored_clusters=true&amp;enable_snippets=true&amp;salary=&amp;only_with_salary=true&amp;search_field=name&amp;text=not+%28company_name%3A%D0%96%D0%AD%D0%A3*+OR+%D0%BC%D1%83%D0%B7%D0%B5%D0%B9*OR+%D0%BA%D0%BE%D0%BB%D0%BB%D0%B5%D0%B4%D0%B6*OR+%D0%BB%D0%B8%D1%86%D0%B5%D0%B9*+OR+%D1%83%D0%BD%D0%B8%D0%B2%D0%B5%D1%80%D1%81%D0%B8%D1%82%D0%B5%D1%82*+OR+%D0%B8%D0%BD%D1%81%D1%82%D0%B8%D1%82%D1%83%D1%82*+OR+%D0%B4%D0%BE%D0%BC-%D0%B8%D0%BD%D1%82%D0%B5%D1%80%D0%BD%D0%B0%D1%82*%29name%3A%21</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;industry=5&amp;industry=42&amp;ored_clusters=true&amp;items_on_page=100&amp;enable_snippets=true&amp;only_with_salary=true&amp;st=searchVacancy&amp;search_field=name&amp;text=NOT+%28грузчик+OR+комплектовщик%29+AND+!</t>
+  </si>
+  <si>
+    <t>Кладовщик,B84,urlForStoreKpr;Слесарь-сантехник,B145,urlForSlesar;Официант,B267,urlForProf</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living_or_relocation&amp;age_to=60&amp;gender=unknown&amp;clusters=true&amp;exp_period=all_time&amp;items_on_page=100&amp;logic=normal&amp;no_magic=true&amp;order_by=relevance&amp;ored_clusters=true&amp;search_period=30&amp;pos=position&amp;text=!</t>
   </si>
 </sst>
 </file>
@@ -568,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -646,40 +641,40 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
+      <c r="B7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>48</v>
@@ -687,60 +682,47 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="14.25" customHeight="1">
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="2:2" ht="14.25" customHeight="1">
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1706,19 +1688,21 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId3"/>
+    <hyperlink ref="B15" display="https://rabota.by/search/resume?text=&quot;Подбор+персонала&quot;+AND+Рекрутинг+AND+Recruiter&amp;logic=normal&amp;pos=education&amp;exp_period=all_time&amp;exp_company_size=any&amp;exp_industry=any&amp;area=1004&amp;relocation=living_or_relocation&amp;salary_from=&amp;salary_to=&amp;currency_code=BYR&amp;ed"/>
+    <hyperlink ref="B12" r:id="rId4"/>
+    <hyperlink ref="B14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
correct fill DB after Спрос
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Уборщик помещений,B84,urlKladVac;Уборщик территории,B145,urlEconVac;Прачка,B23,urlAccVac</t>
+  </si>
+  <si>
+    <t>HH_access_token</t>
+  </si>
+  <si>
+    <t>ONRJ8FH59MTVFR44CL7TLRFK5A2QD8BEG9RU7PVNH05O0PD7EA7IBPHV0II9OM3P</t>
+  </si>
+  <si>
+    <t>Токен для сервиса HH.ru. Используется в API запросах</t>
+  </si>
+  <si>
+    <t>Слесарь-сантехник,B145,urlForSlesar</t>
   </si>
 </sst>
 </file>
@@ -604,7 +616,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -672,7 +684,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
         <v>32</v>
@@ -688,7 +710,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
fix algoritm with exception company by words from Config.xslx
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -237,19 +237,34 @@
     <t>urlDeveloper</t>
   </si>
   <si>
+    <t>Удалять вакансии от ИП и УП? True - удалять; False - Оставлять</t>
+  </si>
+  <si>
+    <t>Remove_IP_UP</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/vacancy?schedule=fullDay&amp;clusters=true&amp;area=1002&amp;area=2237&amp;professional_role=44&amp;professional_role=45&amp;professional_role=46&amp;professional_role=48&amp;professional_role=49&amp;professional_role=80&amp;professional_role=38&amp;professional_role=69&amp;professional_role=30&amp;professional_role=108&amp;professional_role=67&amp;professional_role=142&amp;professional_role=16&amp;ored_clusters=true&amp;enable_snippets=true&amp;only_with_salary=true&amp;salary=&amp;text=%D0%BD%D0%B0%D1%87%D0%B0%D0%BB%D1%8C%D0%BD%D0%B8%D0%BA+%D0%BE%D1%82%D0%B4%D0%B5%D0%BB%D0%B0</t>
+  </si>
+  <si>
+    <t>Продавец,B23,urlForSalesAss</t>
+  </si>
+  <si>
+    <t>resumeURL_copy</t>
+  </si>
+  <si>
+    <t>https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living&amp;age_to=60&amp;gender=unknown&amp;clusters=true&amp;exp_period=all_time&amp;items_on_page=100&amp;logic=normal&amp;no_magic=true&amp;order_by=relevance&amp;ored_clusters=true&amp;search_period=30&amp;pos=position&amp;text=!</t>
+  </si>
+  <si>
     <t>True</t>
   </si>
   <si>
-    <t>Удалять вакансии от ИП и УП? True - удалять; False - Оставлять</t>
-  </si>
-  <si>
-    <t>Remove_IP_UP</t>
-  </si>
-  <si>
-    <t>https://rabota.by/search/vacancy?schedule=fullDay&amp;clusters=true&amp;area=1002&amp;area=2237&amp;professional_role=44&amp;professional_role=45&amp;professional_role=46&amp;professional_role=48&amp;professional_role=49&amp;professional_role=80&amp;professional_role=38&amp;professional_role=69&amp;professional_role=30&amp;professional_role=108&amp;professional_role=67&amp;professional_role=142&amp;professional_role=16&amp;ored_clusters=true&amp;enable_snippets=true&amp;only_with_salary=true&amp;salary=&amp;text=%D0%BD%D0%B0%D1%87%D0%B0%D0%BB%D1%8C%D0%BD%D0%B8%D0%BA+%D0%BE%D1%82%D0%B4%D0%B5%D0%BB%D0%B0</t>
-  </si>
-  <si>
-    <t>начальник отдела,B23,urlDeveloper</t>
+    <t>Исключить компании, содержащие слова</t>
+  </si>
+  <si>
+    <t>RemoveCompany</t>
+  </si>
+  <si>
+    <t>поликлиника;больница;спартак;рапа</t>
   </si>
 </sst>
 </file>
@@ -642,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -731,177 +746,187 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>77</v>
       </c>
     </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1">
-      <c r="A12" t="s">
+    <row r="13" spans="1:26" ht="15" customHeight="1">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" t="s">
+    <row r="16" spans="1:26" ht="15" customHeight="1">
+      <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="6" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
       <c r="B19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="A22" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>55</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B28" t="s">
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
+      <c r="B31" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="34" spans="2:2" ht="14.25" customHeight="1"/>
-    <row r="35" spans="2:2" ht="14.25" customHeight="1">
-      <c r="B35" t="s">
+    <row r="35" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="2:2" ht="14.25" customHeight="1"/>
@@ -1867,18 +1892,24 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B12" display="https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;industry=5&amp;industry=42&amp;specialization=21.563&amp;specialization=21.564&amp;ored_clusters=true&amp;items_on_page=100&amp;enable_snippets=true&amp;only_with_salary=true&amp;st=searchVacancy&amp;search_field=name&amp;text=NOT+%28груз"/>
-    <hyperlink ref="B16" display="https://rabota.by/search/resume?text=&quot;Подбор+персонала&quot;+OR+Рекрутинг+OR+Recruiter&amp;logic=normal&amp;pos=education&amp;exp_period=all_time&amp;exp_company_size=any&amp;exp_industry=any&amp;area=1004&amp;relocation=living_or_relocation&amp;salary_from=&amp;salary_to=&amp;currency_code=BYR&amp;educ"/>
-    <hyperlink ref="B13" display="https://rabota.by/search/vacancy?area=1002&amp;items_on_page=100&amp;search_field=name&amp;professional_role=131&amp;industry=5&amp;industry=27&amp;industry=41&amp;specialization=29.545&amp;only_with_salary=true&amp;clusters=true&amp;ored_clusters=true&amp;enable_snippets=true&amp;text=Укладчик-упаковщ"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-    <hyperlink ref="B14" display="https://rabota.by/search/vacancy?area=1002&amp;search_field=name&amp;search_field=company_name&amp;only_with_salary=true&amp;clusters=true&amp;items_on_page=100&amp;no_magic=true&amp;ored_clusters=true&amp;enable_snippets=true&amp;text=not+(company_name:ЖЭУ* OR музей*OR колледж*OR лицей* OR"/>
-    <hyperlink ref="B26" r:id="rId3"/>
-    <hyperlink ref="B17" display="https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living_or_relocation&amp;ag"/>
-    <hyperlink ref="B15" display="https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living_or_relocation&amp;ag"/>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B13" display="https://rabota.by/search/vacancy?clusters=true&amp;area=1002&amp;industry=5&amp;industry=42&amp;specialization=21.563&amp;specialization=21.564&amp;ored_clusters=true&amp;items_on_page=100&amp;enable_snippets=true&amp;only_with_salary=true&amp;st=searchVacancy&amp;search_field=name&amp;text=NOT+%28груз"/>
+    <hyperlink ref="B17" display="https://rabota.by/search/resume?text=&quot;Подбор+персонала&quot;+OR+Рекрутинг+OR+Recruiter&amp;logic=normal&amp;pos=education&amp;exp_period=all_time&amp;exp_company_size=any&amp;exp_industry=any&amp;area=1004&amp;relocation=living_or_relocation&amp;salary_from=&amp;salary_to=&amp;currency_code=BYR&amp;educ"/>
+    <hyperlink ref="B14" display="https://rabota.by/search/vacancy?area=1002&amp;items_on_page=100&amp;search_field=name&amp;professional_role=131&amp;industry=5&amp;industry=27&amp;industry=41&amp;specialization=29.545&amp;only_with_salary=true&amp;clusters=true&amp;ored_clusters=true&amp;enable_snippets=true&amp;text=Укладчик-упаковщ"/>
+    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B15" display="https://rabota.by/search/vacancy?area=1002&amp;search_field=name&amp;search_field=company_name&amp;only_with_salary=true&amp;clusters=true&amp;items_on_page=100&amp;no_magic=true&amp;ored_clusters=true&amp;enable_snippets=true&amp;text=not+(company_name:ЖЭУ* OR музей*OR колледж*OR лицей* OR"/>
+    <hyperlink ref="B27" r:id="rId3"/>
+    <hyperlink ref="B18" display="https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living_or_relocation&amp;ag"/>
+    <hyperlink ref="B16" display="https://rabota.by/search/resume?area=1002&amp;clusters=true&amp;currency_code=BYR&amp;exp_period=all_time&amp;items_on_page=100&amp;label=only_with_salary&amp;logic=normal&amp;no_magichttps://rabota.by/search/resume?area=1002&amp;label=only_with_salary&amp;relocation=living&amp;age_to=60&amp;gender"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>